<commit_message>
grpc article test finished
</commit_message>
<xml_diff>
--- a/Testaufbau/BenchmarkResults/BenchmarkResults.xlsx
+++ b/Testaufbau/BenchmarkResults/BenchmarkResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studium\8. Semester\Bachelorarbeit\TestaufbauGit\Testaufbau\Testaufbau\BenchmarkResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85784861-828F-4384-84A7-743D8B55768B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95DD5093-73BC-458D-9908-1C3A625205A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="2890" windowWidth="18900" windowHeight="11860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RestClient.Benchmark.GetArticle" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="171">
   <si>
     <t>Method</t>
   </si>
@@ -344,6 +344,195 @@
   </si>
   <si>
     <t>TotalTime: 26:29</t>
+  </si>
+  <si>
+    <t>Mit ToListAsync() bei OrdersWithOrderItems</t>
+  </si>
+  <si>
+    <t>1.724 ms</t>
+  </si>
+  <si>
+    <t>0.0173 ms</t>
+  </si>
+  <si>
+    <t>0.0145 ms</t>
+  </si>
+  <si>
+    <t>3.678 ms</t>
+  </si>
+  <si>
+    <t>0.0533 ms</t>
+  </si>
+  <si>
+    <t>0.0472 ms</t>
+  </si>
+  <si>
+    <t>3.505 ms</t>
+  </si>
+  <si>
+    <t>0.0244 ms</t>
+  </si>
+  <si>
+    <t>0.0488 ms</t>
+  </si>
+  <si>
+    <t>2.042 ms</t>
+  </si>
+  <si>
+    <t>0.0187 ms</t>
+  </si>
+  <si>
+    <t>0.0146 ms</t>
+  </si>
+  <si>
+    <t>1.827 ms</t>
+  </si>
+  <si>
+    <t>0.0297 ms</t>
+  </si>
+  <si>
+    <t>0.0278 ms</t>
+  </si>
+  <si>
+    <t>3.684 ms</t>
+  </si>
+  <si>
+    <t>0.0607 ms</t>
+  </si>
+  <si>
+    <t>0.0568 ms</t>
+  </si>
+  <si>
+    <t>19.404 ms</t>
+  </si>
+  <si>
+    <t>0.3811 ms</t>
+  </si>
+  <si>
+    <t>0.3565 ms</t>
+  </si>
+  <si>
+    <t>2.285 ms</t>
+  </si>
+  <si>
+    <t>0.0453 ms</t>
+  </si>
+  <si>
+    <t>0.0745 ms</t>
+  </si>
+  <si>
+    <t>2.535 ms</t>
+  </si>
+  <si>
+    <t>0.0477 ms</t>
+  </si>
+  <si>
+    <t>0.0446 ms</t>
+  </si>
+  <si>
+    <t>3.860 ms</t>
+  </si>
+  <si>
+    <t>0.0499 ms</t>
+  </si>
+  <si>
+    <t>0.0416 ms</t>
+  </si>
+  <si>
+    <t>175.584 ms</t>
+  </si>
+  <si>
+    <t>2.0780 ms</t>
+  </si>
+  <si>
+    <t>1.8421 ms</t>
+  </si>
+  <si>
+    <t>3.450 ms</t>
+  </si>
+  <si>
+    <t>0.0414 ms</t>
+  </si>
+  <si>
+    <t>0.0367 ms</t>
+  </si>
+  <si>
+    <t>9.120 ms</t>
+  </si>
+  <si>
+    <t>0.1811 ms</t>
+  </si>
+  <si>
+    <t>0.3860 ms</t>
+  </si>
+  <si>
+    <t>5.140 ms</t>
+  </si>
+  <si>
+    <t>0.0612 ms</t>
+  </si>
+  <si>
+    <t>0.0543 ms</t>
+  </si>
+  <si>
+    <t>1,747.136 ms</t>
+  </si>
+  <si>
+    <t>17.4654 ms</t>
+  </si>
+  <si>
+    <t>16.3371 ms</t>
+  </si>
+  <si>
+    <t>15.707 ms</t>
+  </si>
+  <si>
+    <t>0.2982 ms</t>
+  </si>
+  <si>
+    <t>0.6546 ms</t>
+  </si>
+  <si>
+    <t>68.935 ms</t>
+  </si>
+  <si>
+    <t>1.3413 ms</t>
+  </si>
+  <si>
+    <t>1.3774 ms</t>
+  </si>
+  <si>
+    <t>15.177 ms</t>
+  </si>
+  <si>
+    <t>0.2966 ms</t>
+  </si>
+  <si>
+    <t>0.2774 ms</t>
+  </si>
+  <si>
+    <t>17,406.282 ms</t>
+  </si>
+  <si>
+    <t>72.2577 ms</t>
+  </si>
+  <si>
+    <t>67.5899 ms</t>
+  </si>
+  <si>
+    <t>132.789 ms</t>
+  </si>
+  <si>
+    <t>2.2503 ms</t>
+  </si>
+  <si>
+    <t>4.1711 ms</t>
+  </si>
+  <si>
+    <t>TotalTime: 14:46</t>
+  </si>
+  <si>
+    <t>gRPC:</t>
   </si>
 </sst>
 </file>
@@ -1197,10 +1386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:H31"/>
+  <dimension ref="A3:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1639,6 +1828,11 @@
         <v>106</v>
       </c>
     </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>108</v>
+      </c>
+    </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>90</v>
@@ -1727,9 +1921,374 @@
         <v>107</v>
       </c>
     </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>3</v>
+      </c>
+      <c r="E35" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37">
+        <v>10</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38">
+        <v>100</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39">
+        <v>1000</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40">
+        <v>10000</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42">
+        <v>10</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43">
+        <v>100</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44">
+        <v>1000</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>11</v>
+      </c>
+      <c r="B45">
+        <v>10000</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>16</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47">
+        <v>10</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>16</v>
+      </c>
+      <c r="B48">
+        <v>100</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>16</v>
+      </c>
+      <c r="B49">
+        <v>1000</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>16</v>
+      </c>
+      <c r="B50">
+        <v>10000</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>21</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>21</v>
+      </c>
+      <c r="B52">
+        <v>10</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>21</v>
+      </c>
+      <c r="B53">
+        <v>100</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>21</v>
+      </c>
+      <c r="B54">
+        <v>1000</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>21</v>
+      </c>
+      <c r="B55">
+        <v>10000</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:F24">
-    <sortCondition ref="A5:A24" customList="GetArticles,GetReducedArticles,GetArticlesWithPriceChatty,GetArticlesWithPriceBulky"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A36:E55">
+    <sortCondition ref="A36:A55" customList="GetArticles,GetReducedArticles,GetArticlesWithPriceChatty,GetArticlesWithPriceBulky"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
grpc order test fehlt noch
</commit_message>
<xml_diff>
--- a/Testaufbau/BenchmarkResults/BenchmarkResults.xlsx
+++ b/Testaufbau/BenchmarkResults/BenchmarkResults.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studium\8. Semester\Bachelorarbeit\TestaufbauGit\Testaufbau\Testaufbau\BenchmarkResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95DD5093-73BC-458D-9908-1C3A625205A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760D0BD1-2D1C-4C43-A714-FB6A6971255A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="2890" windowWidth="18900" windowHeight="11860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25420" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="RestClient.Benchmark.GetArticle" sheetId="1" r:id="rId1"/>
+    <sheet name="BenchmarkResults" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="235">
   <si>
     <t>Method</t>
   </si>
@@ -533,6 +533,198 @@
   </si>
   <si>
     <t>gRPC:</t>
+  </si>
+  <si>
+    <t>GraphQl</t>
+  </si>
+  <si>
+    <t>1.084 ms</t>
+  </si>
+  <si>
+    <t>0.0112 ms</t>
+  </si>
+  <si>
+    <t>0.0105 ms</t>
+  </si>
+  <si>
+    <t>1.058 ms</t>
+  </si>
+  <si>
+    <t>0.0205 ms</t>
+  </si>
+  <si>
+    <t>GetArticlesWithPrice</t>
+  </si>
+  <si>
+    <t>1.919 ms</t>
+  </si>
+  <si>
+    <t>0.0268 ms</t>
+  </si>
+  <si>
+    <t>0.0251 ms</t>
+  </si>
+  <si>
+    <t>1.185 ms</t>
+  </si>
+  <si>
+    <t>0.0110 ms</t>
+  </si>
+  <si>
+    <t>0.0092 ms</t>
+  </si>
+  <si>
+    <t>1.107 ms</t>
+  </si>
+  <si>
+    <t>0.0217 ms</t>
+  </si>
+  <si>
+    <t>0.0203 ms</t>
+  </si>
+  <si>
+    <t>9.371 ms</t>
+  </si>
+  <si>
+    <t>0.1696 ms</t>
+  </si>
+  <si>
+    <t>0.1586 ms</t>
+  </si>
+  <si>
+    <t>2.165 ms</t>
+  </si>
+  <si>
+    <t>0.0312 ms</t>
+  </si>
+  <si>
+    <t>0.0277 ms</t>
+  </si>
+  <si>
+    <t>1.557 ms</t>
+  </si>
+  <si>
+    <t>0.0102 ms</t>
+  </si>
+  <si>
+    <t>0.0079 ms</t>
+  </si>
+  <si>
+    <t>84.642 ms</t>
+  </si>
+  <si>
+    <t>0.6412 ms</t>
+  </si>
+  <si>
+    <t>0.5355 ms</t>
+  </si>
+  <si>
+    <t>11.177 ms</t>
+  </si>
+  <si>
+    <t>0.0864 ms</t>
+  </si>
+  <si>
+    <t>0.0766 ms</t>
+  </si>
+  <si>
+    <t>6.147 ms</t>
+  </si>
+  <si>
+    <t>0.0639 ms</t>
+  </si>
+  <si>
+    <t>0.0534 ms</t>
+  </si>
+  <si>
+    <t>820.182 ms</t>
+  </si>
+  <si>
+    <t>8.7843 ms</t>
+  </si>
+  <si>
+    <t>7.3352 ms</t>
+  </si>
+  <si>
+    <t>100.656 ms</t>
+  </si>
+  <si>
+    <t>1.6371 ms</t>
+  </si>
+  <si>
+    <t>1.4512 ms</t>
+  </si>
+  <si>
+    <t>52.337 ms</t>
+  </si>
+  <si>
+    <t>0.6480 ms</t>
+  </si>
+  <si>
+    <t>0.6061 ms</t>
+  </si>
+  <si>
+    <t>8,402.723 ms</t>
+  </si>
+  <si>
+    <t>57.3451 ms</t>
+  </si>
+  <si>
+    <t>50.8349 ms</t>
+  </si>
+  <si>
+    <t>NumberOfOrders</t>
+  </si>
+  <si>
+    <t>3.247 ms</t>
+  </si>
+  <si>
+    <t>0.0645 ms</t>
+  </si>
+  <si>
+    <t>0.1179 ms</t>
+  </si>
+  <si>
+    <t>36.664 ms</t>
+  </si>
+  <si>
+    <t>0.7296 ms</t>
+  </si>
+  <si>
+    <t>0.7165 ms</t>
+  </si>
+  <si>
+    <t>313.824 ms</t>
+  </si>
+  <si>
+    <t>5.9499 ms</t>
+  </si>
+  <si>
+    <t>6.1101 ms</t>
+  </si>
+  <si>
+    <t>3,281.162 ms</t>
+  </si>
+  <si>
+    <t>25.7327 ms</t>
+  </si>
+  <si>
+    <t>24.0704 ms</t>
+  </si>
+  <si>
+    <t>64,717.229 ms</t>
+  </si>
+  <si>
+    <t>122.5409 ms</t>
+  </si>
+  <si>
+    <t>114.6249 ms</t>
+  </si>
+  <si>
+    <t>REST</t>
+  </si>
+  <si>
+    <t>Grpc</t>
   </si>
 </sst>
 </file>
@@ -1386,10 +1578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:H55"/>
+  <dimension ref="A3:N81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1398,14 +1590,18 @@
     <col min="2" max="2" width="20.6328125" customWidth="1"/>
     <col min="3" max="6" width="20.6328125" style="2" customWidth="1"/>
     <col min="8" max="8" width="34" style="4" customWidth="1"/>
+    <col min="11" max="11" width="21.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1424,8 +1620,20 @@
       <c r="F4" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="M4" t="s">
+        <v>234</v>
+      </c>
+      <c r="N4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1444,8 +1652,20 @@
       <c r="F5" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="N5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1464,8 +1684,20 @@
       <c r="F6" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K6">
+        <v>10</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="N6" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1484,8 +1716,20 @@
       <c r="F7" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K7">
+        <v>100</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="N7" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1504,8 +1748,20 @@
       <c r="F8" s="1" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K8">
+        <v>1000</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="N8" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1524,8 +1780,20 @@
       <c r="F9" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K9">
+        <v>10000</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="N9" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1545,7 +1813,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1564,8 +1832,11 @@
       <c r="F11" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1584,8 +1855,20 @@
       <c r="F12" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="M12" t="s">
+        <v>234</v>
+      </c>
+      <c r="N12" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1604,8 +1887,20 @@
       <c r="F13" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="N13" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1624,8 +1919,20 @@
       <c r="F14" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K14">
+        <v>10</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="N14" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1644,8 +1951,20 @@
       <c r="F15" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="K15">
+        <v>100</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="N15" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -1664,8 +1983,20 @@
       <c r="F16" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="K16">
+        <v>1000</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="N16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1684,8 +2015,20 @@
       <c r="F17" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="K17">
+        <v>10000</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="N17" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1704,8 +2047,9 @@
       <c r="F18" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -1724,8 +2068,11 @@
       <c r="F19" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="K19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1744,8 +2091,20 @@
       <c r="F20" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="K20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L20" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="M20" t="s">
+        <v>234</v>
+      </c>
+      <c r="N20" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -1764,8 +2123,20 @@
       <c r="F21" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="N21" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1784,8 +2155,20 @@
       <c r="F22" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="K22">
+        <v>10</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="N22" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1804,8 +2187,20 @@
       <c r="F23" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="K23">
+        <v>100</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="N23" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1827,13 +2222,39 @@
       <c r="H24" s="4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="K24">
+        <v>1000</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="N24" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="K25">
+        <v>10000</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="N25" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>90</v>
       </c>
@@ -1849,8 +2270,11 @@
       <c r="E27" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="K27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>90</v>
       </c>
@@ -1866,8 +2290,20 @@
       <c r="E28" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="K28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="M28" t="s">
+        <v>234</v>
+      </c>
+      <c r="N28" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>90</v>
       </c>
@@ -1883,8 +2319,20 @@
       <c r="E29" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="N29" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>90</v>
       </c>
@@ -1900,8 +2348,20 @@
       <c r="E30" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="K30">
+        <v>10</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="N30" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>90</v>
       </c>
@@ -1920,13 +2380,53 @@
       <c r="H31" s="4" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K31">
+        <v>100</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="N31" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="K32">
+        <v>1000</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="N32" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="K33">
+        <v>10000</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="N33" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -1943,7 +2443,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>6</v>
       </c>
@@ -1960,7 +2460,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -1977,7 +2477,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -1994,7 +2494,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>6</v>
       </c>
@@ -2011,7 +2511,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -2028,7 +2528,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>11</v>
       </c>
@@ -2045,7 +2545,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -2062,7 +2562,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>11</v>
       </c>
@@ -2079,7 +2579,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>11</v>
       </c>
@@ -2096,7 +2596,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>11</v>
       </c>
@@ -2113,7 +2613,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>16</v>
       </c>
@@ -2130,7 +2630,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>16</v>
       </c>
@@ -2147,7 +2647,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>16</v>
       </c>
@@ -2286,9 +2786,388 @@
         <v>169</v>
       </c>
     </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>0</v>
+      </c>
+      <c r="B59" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" t="s">
+        <v>2</v>
+      </c>
+      <c r="D59" t="s">
+        <v>3</v>
+      </c>
+      <c r="E59" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A60" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60" t="s">
+        <v>172</v>
+      </c>
+      <c r="D60" t="s">
+        <v>173</v>
+      </c>
+      <c r="E60" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>6</v>
+      </c>
+      <c r="B61">
+        <v>10</v>
+      </c>
+      <c r="C61" t="s">
+        <v>181</v>
+      </c>
+      <c r="D61" t="s">
+        <v>182</v>
+      </c>
+      <c r="E61" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62">
+        <v>100</v>
+      </c>
+      <c r="C62" t="s">
+        <v>190</v>
+      </c>
+      <c r="D62" t="s">
+        <v>191</v>
+      </c>
+      <c r="E62" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63">
+        <v>1000</v>
+      </c>
+      <c r="C63" t="s">
+        <v>199</v>
+      </c>
+      <c r="D63" t="s">
+        <v>200</v>
+      </c>
+      <c r="E63" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>6</v>
+      </c>
+      <c r="B64">
+        <v>10000</v>
+      </c>
+      <c r="C64" t="s">
+        <v>208</v>
+      </c>
+      <c r="D64" t="s">
+        <v>209</v>
+      </c>
+      <c r="E64" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>11</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65" t="s">
+        <v>175</v>
+      </c>
+      <c r="D65" t="s">
+        <v>176</v>
+      </c>
+      <c r="E65" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>11</v>
+      </c>
+      <c r="B66">
+        <v>10</v>
+      </c>
+      <c r="C66" t="s">
+        <v>184</v>
+      </c>
+      <c r="D66" t="s">
+        <v>185</v>
+      </c>
+      <c r="E66" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>11</v>
+      </c>
+      <c r="B67">
+        <v>100</v>
+      </c>
+      <c r="C67" t="s">
+        <v>193</v>
+      </c>
+      <c r="D67" t="s">
+        <v>194</v>
+      </c>
+      <c r="E67" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>11</v>
+      </c>
+      <c r="B68">
+        <v>1000</v>
+      </c>
+      <c r="C68" t="s">
+        <v>202</v>
+      </c>
+      <c r="D68" t="s">
+        <v>203</v>
+      </c>
+      <c r="E68" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>11</v>
+      </c>
+      <c r="B69">
+        <v>10000</v>
+      </c>
+      <c r="C69" t="s">
+        <v>211</v>
+      </c>
+      <c r="D69" t="s">
+        <v>212</v>
+      </c>
+      <c r="E69" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>177</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70" t="s">
+        <v>178</v>
+      </c>
+      <c r="D70" t="s">
+        <v>179</v>
+      </c>
+      <c r="E70" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71" t="s">
+        <v>177</v>
+      </c>
+      <c r="B71">
+        <v>10</v>
+      </c>
+      <c r="C71" t="s">
+        <v>187</v>
+      </c>
+      <c r="D71" t="s">
+        <v>188</v>
+      </c>
+      <c r="E71" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72" t="s">
+        <v>177</v>
+      </c>
+      <c r="B72">
+        <v>100</v>
+      </c>
+      <c r="C72" t="s">
+        <v>196</v>
+      </c>
+      <c r="D72" t="s">
+        <v>197</v>
+      </c>
+      <c r="E72" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>177</v>
+      </c>
+      <c r="B73">
+        <v>1000</v>
+      </c>
+      <c r="C73" t="s">
+        <v>205</v>
+      </c>
+      <c r="D73" t="s">
+        <v>206</v>
+      </c>
+      <c r="E73" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>177</v>
+      </c>
+      <c r="B74">
+        <v>10000</v>
+      </c>
+      <c r="C74" t="s">
+        <v>214</v>
+      </c>
+      <c r="D74" t="s">
+        <v>215</v>
+      </c>
+      <c r="E74" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>0</v>
+      </c>
+      <c r="B76" t="s">
+        <v>217</v>
+      </c>
+      <c r="C76" t="s">
+        <v>2</v>
+      </c>
+      <c r="D76" t="s">
+        <v>3</v>
+      </c>
+      <c r="E76" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>90</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77" t="s">
+        <v>218</v>
+      </c>
+      <c r="D77" t="s">
+        <v>219</v>
+      </c>
+      <c r="E77" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>90</v>
+      </c>
+      <c r="B78">
+        <v>10</v>
+      </c>
+      <c r="C78" t="s">
+        <v>221</v>
+      </c>
+      <c r="D78" t="s">
+        <v>222</v>
+      </c>
+      <c r="E78" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>90</v>
+      </c>
+      <c r="B79">
+        <v>100</v>
+      </c>
+      <c r="C79" t="s">
+        <v>224</v>
+      </c>
+      <c r="D79" t="s">
+        <v>225</v>
+      </c>
+      <c r="E79" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>90</v>
+      </c>
+      <c r="B80">
+        <v>1000</v>
+      </c>
+      <c r="C80" t="s">
+        <v>227</v>
+      </c>
+      <c r="D80" t="s">
+        <v>228</v>
+      </c>
+      <c r="E80" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>90</v>
+      </c>
+      <c r="B81">
+        <v>10000</v>
+      </c>
+      <c r="C81" t="s">
+        <v>230</v>
+      </c>
+      <c r="D81" t="s">
+        <v>231</v>
+      </c>
+      <c r="E81" t="s">
+        <v>232</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A36:E55">
-    <sortCondition ref="A36:A55" customList="GetArticles,GetReducedArticles,GetArticlesWithPriceChatty,GetArticlesWithPriceBulky"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A60:E74">
+    <sortCondition ref="A60:A74" customList="GetArticles,GetReducedArticles,GetArticlesWithPriceChatty,GetArticlesWithPriceBulky"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
graphql powerup mit data loader
</commit_message>
<xml_diff>
--- a/Testaufbau/BenchmarkResults/BenchmarkResults.xlsx
+++ b/Testaufbau/BenchmarkResults/BenchmarkResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studium\8. Semester\Bachelorarbeit\TestaufbauGit\Testaufbau\Testaufbau\BenchmarkResults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA98CD3-EE81-42AC-B0C0-46523F3BD771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BCD7005-94A5-4509-A8DA-2B33EABE6B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12600" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12600" yWindow="0" windowWidth="12600" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BenchmarkResults" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1044" uniqueCount="643">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="684">
   <si>
     <t>Method</t>
   </si>
@@ -1949,6 +1949,129 @@
   </si>
   <si>
     <t>Verschlechterung durch "chatty" verarbeitung anstelle von einem dedizierten Endpunkt</t>
+  </si>
+  <si>
+    <t>1.069 ms</t>
+  </si>
+  <si>
+    <t>0.0237 ms</t>
+  </si>
+  <si>
+    <t>1.010 ms</t>
+  </si>
+  <si>
+    <t>0.0154 ms</t>
+  </si>
+  <si>
+    <t>0.0129 ms</t>
+  </si>
+  <si>
+    <t>1.206 ms</t>
+  </si>
+  <si>
+    <t>0.0191 ms</t>
+  </si>
+  <si>
+    <t>0.0234 ms</t>
+  </si>
+  <si>
+    <t>1.173 ms</t>
+  </si>
+  <si>
+    <t>0.0213 ms</t>
+  </si>
+  <si>
+    <t>0.0209 ms</t>
+  </si>
+  <si>
+    <t>1.079 ms</t>
+  </si>
+  <si>
+    <t>0.0098 ms</t>
+  </si>
+  <si>
+    <t>0.0076 ms</t>
+  </si>
+  <si>
+    <t>1.930 ms</t>
+  </si>
+  <si>
+    <t>0.0091 ms</t>
+  </si>
+  <si>
+    <t>2.161 ms</t>
+  </si>
+  <si>
+    <t>0.0426 ms</t>
+  </si>
+  <si>
+    <t>0.0456 ms</t>
+  </si>
+  <si>
+    <t>1.562 ms</t>
+  </si>
+  <si>
+    <t>0.0264 ms</t>
+  </si>
+  <si>
+    <t>8.952 ms</t>
+  </si>
+  <si>
+    <t>0.1757 ms</t>
+  </si>
+  <si>
+    <t>0.1805 ms</t>
+  </si>
+  <si>
+    <t>11.651 ms</t>
+  </si>
+  <si>
+    <t>0.1233 ms</t>
+  </si>
+  <si>
+    <t>6.254 ms</t>
+  </si>
+  <si>
+    <t>0.1079 ms</t>
+  </si>
+  <si>
+    <t>0.0901 ms</t>
+  </si>
+  <si>
+    <t>71.041 ms</t>
+  </si>
+  <si>
+    <t>0.4321 ms</t>
+  </si>
+  <si>
+    <t>0.4042 ms</t>
+  </si>
+  <si>
+    <t>103.338 ms</t>
+  </si>
+  <si>
+    <t>0.7706 ms</t>
+  </si>
+  <si>
+    <t>0.6016 ms</t>
+  </si>
+  <si>
+    <t>54.928 ms</t>
+  </si>
+  <si>
+    <t>0.9212 ms</t>
+  </si>
+  <si>
+    <t>0.7692 ms</t>
+  </si>
+  <si>
+    <t>725.548 ms</t>
+  </si>
+  <si>
+    <t>14.2297 ms</t>
+  </si>
+  <si>
+    <t>21.2983 ms</t>
   </si>
 </sst>
 </file>
@@ -2834,7 +2957,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2967,6 +3090,7 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3324,8 +3448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J59" sqref="J59"/>
+    <sheetView tabSelected="1" topLeftCell="P49" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" outlineLevelCol="1" x14ac:dyDescent="0.35"/>
@@ -3346,9 +3470,11 @@
     <col min="16" max="16" width="15.7265625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="17" max="17" width="12.7265625" style="9" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="11.26953125" customWidth="1" outlineLevel="1"/>
-    <col min="20" max="22" width="10.90625" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="23" width="12.81640625" style="4" customWidth="1"/>
-    <col min="24" max="24" width="14.26953125" style="9" customWidth="1"/>
+    <col min="20" max="21" width="10.90625" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="28" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="15.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.7265625" style="9" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.35">
@@ -6063,7 +6189,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B65" s="68"/>
       <c r="C65" s="69"/>
       <c r="I65" s="68"/>
@@ -6073,7 +6199,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:26" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A66" s="51" t="s">
         <v>249</v>
       </c>
@@ -6092,7 +6218,7 @@
       <c r="N66" s="55"/>
       <c r="O66" s="55"/>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A67" s="58" t="s">
         <v>0</v>
       </c>
@@ -6138,8 +6264,23 @@
       <c r="S67" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="V67" t="s">
+        <v>0</v>
+      </c>
+      <c r="W67" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="X67" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y67" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z67" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A68" s="58" t="s">
         <v>6</v>
       </c>
@@ -6185,8 +6326,23 @@
       <c r="S68" s="1" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="V68" t="s">
+        <v>6</v>
+      </c>
+      <c r="W68" s="4">
+        <v>1</v>
+      </c>
+      <c r="X68" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="Y68" t="s">
+        <v>361</v>
+      </c>
+      <c r="Z68" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="69" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A69" s="58" t="s">
         <v>6</v>
       </c>
@@ -6232,8 +6388,23 @@
       <c r="S69" s="1" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="V69" t="s">
+        <v>6</v>
+      </c>
+      <c r="W69" s="4">
+        <v>10</v>
+      </c>
+      <c r="X69" s="9" t="s">
+        <v>651</v>
+      </c>
+      <c r="Y69" t="s">
+        <v>652</v>
+      </c>
+      <c r="Z69" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="70" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A70" s="58" t="s">
         <v>6</v>
       </c>
@@ -6279,8 +6450,23 @@
       <c r="S70" s="1" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="V70" t="s">
+        <v>6</v>
+      </c>
+      <c r="W70" s="4">
+        <v>100</v>
+      </c>
+      <c r="X70" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="Y70" t="s">
+        <v>660</v>
+      </c>
+      <c r="Z70" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="71" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A71" s="58" t="s">
         <v>6</v>
       </c>
@@ -6326,8 +6512,23 @@
       <c r="S71" s="1" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="V71" t="s">
+        <v>6</v>
+      </c>
+      <c r="W71" s="4">
+        <v>1000</v>
+      </c>
+      <c r="X71" s="9" t="s">
+        <v>667</v>
+      </c>
+      <c r="Y71" t="s">
+        <v>668</v>
+      </c>
+      <c r="Z71" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="72" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A72" s="58" t="s">
         <v>6</v>
       </c>
@@ -6373,8 +6574,23 @@
       <c r="S72" s="1" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="V72" t="s">
+        <v>6</v>
+      </c>
+      <c r="W72" s="4">
+        <v>10000</v>
+      </c>
+      <c r="X72" s="9" t="s">
+        <v>675</v>
+      </c>
+      <c r="Y72" t="s">
+        <v>676</v>
+      </c>
+      <c r="Z72" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="73" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A73" s="58" t="s">
         <v>11</v>
       </c>
@@ -6420,8 +6636,23 @@
       <c r="S73" s="1" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="V73" t="s">
+        <v>11</v>
+      </c>
+      <c r="W73" s="4">
+        <v>1</v>
+      </c>
+      <c r="X73" s="9" t="s">
+        <v>645</v>
+      </c>
+      <c r="Y73" t="s">
+        <v>646</v>
+      </c>
+      <c r="Z73" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="74" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A74" s="58" t="s">
         <v>11</v>
       </c>
@@ -6467,8 +6698,23 @@
       <c r="S74" s="1" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="V74" t="s">
+        <v>11</v>
+      </c>
+      <c r="W74" s="4">
+        <v>10</v>
+      </c>
+      <c r="X74" s="9" t="s">
+        <v>654</v>
+      </c>
+      <c r="Y74" t="s">
+        <v>655</v>
+      </c>
+      <c r="Z74" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="75" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A75" s="58" t="s">
         <v>11</v>
       </c>
@@ -6514,8 +6760,23 @@
       <c r="S75" s="1" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="V75" t="s">
+        <v>11</v>
+      </c>
+      <c r="W75" s="4">
+        <v>100</v>
+      </c>
+      <c r="X75" s="9" t="s">
+        <v>662</v>
+      </c>
+      <c r="Y75" t="s">
+        <v>663</v>
+      </c>
+      <c r="Z75" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="76" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A76" s="58" t="s">
         <v>11</v>
       </c>
@@ -6561,8 +6822,23 @@
       <c r="S76" s="1" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="V76" t="s">
+        <v>11</v>
+      </c>
+      <c r="W76" s="4">
+        <v>1000</v>
+      </c>
+      <c r="X76" s="9" t="s">
+        <v>669</v>
+      </c>
+      <c r="Y76" t="s">
+        <v>670</v>
+      </c>
+      <c r="Z76" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="77" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A77" s="58" t="s">
         <v>11</v>
       </c>
@@ -6608,8 +6884,23 @@
       <c r="S77" s="1" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="V77" t="s">
+        <v>11</v>
+      </c>
+      <c r="W77" s="4">
+        <v>10000</v>
+      </c>
+      <c r="X77" s="9" t="s">
+        <v>678</v>
+      </c>
+      <c r="Y77" t="s">
+        <v>679</v>
+      </c>
+      <c r="Z77" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="78" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A78" s="58" t="s">
         <v>175</v>
       </c>
@@ -6655,8 +6946,23 @@
       <c r="S78" s="1" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="V78" t="s">
+        <v>175</v>
+      </c>
+      <c r="W78" s="4">
+        <v>1</v>
+      </c>
+      <c r="X78" s="9" t="s">
+        <v>648</v>
+      </c>
+      <c r="Y78" t="s">
+        <v>649</v>
+      </c>
+      <c r="Z78" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="79" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A79" s="58" t="s">
         <v>175</v>
       </c>
@@ -6702,8 +7008,23 @@
       <c r="S79" s="1" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="V79" t="s">
+        <v>175</v>
+      </c>
+      <c r="W79" s="4">
+        <v>10</v>
+      </c>
+      <c r="X79" s="9" t="s">
+        <v>657</v>
+      </c>
+      <c r="Y79" t="s">
+        <v>180</v>
+      </c>
+      <c r="Z79" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="80" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A80" s="58" t="s">
         <v>175</v>
       </c>
@@ -6749,8 +7070,23 @@
       <c r="S80" s="1" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="V80" t="s">
+        <v>175</v>
+      </c>
+      <c r="W80" s="4">
+        <v>100</v>
+      </c>
+      <c r="X80" s="9" t="s">
+        <v>664</v>
+      </c>
+      <c r="Y80" t="s">
+        <v>665</v>
+      </c>
+      <c r="Z80" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="81" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A81" s="58" t="s">
         <v>175</v>
       </c>
@@ -6796,8 +7132,23 @@
       <c r="S81" s="1" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="V81" t="s">
+        <v>175</v>
+      </c>
+      <c r="W81" s="4">
+        <v>1000</v>
+      </c>
+      <c r="X81" s="9" t="s">
+        <v>672</v>
+      </c>
+      <c r="Y81" t="s">
+        <v>673</v>
+      </c>
+      <c r="Z81" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="82" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A82" s="58" t="s">
         <v>175</v>
       </c>
@@ -6843,11 +7194,27 @@
       <c r="S82" s="1" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="V82" t="s">
+        <v>175</v>
+      </c>
+      <c r="W82" s="4">
+        <v>10000</v>
+      </c>
+      <c r="X82" s="9" t="s">
+        <v>681</v>
+      </c>
+      <c r="Y82" t="s">
+        <v>682</v>
+      </c>
+      <c r="Z82" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="83" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A83" s="58"/>
-    </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="X83" s="74"/>
+    </row>
+    <row r="84" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A84" s="58" t="s">
         <v>0</v>
       </c>
@@ -6879,7 +7246,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A85" s="58" t="s">
         <v>90</v>
       </c>
@@ -6911,7 +7278,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A86" s="58" t="s">
         <v>90</v>
       </c>
@@ -6943,7 +7310,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A87" s="58" t="s">
         <v>90</v>
       </c>
@@ -6975,7 +7342,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A88" s="58" t="s">
         <v>90</v>
       </c>
@@ -7007,7 +7374,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="89" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A89" s="59" t="s">
         <v>90</v>
       </c>
@@ -7048,16 +7415,16 @@
         <v>547</v>
       </c>
     </row>
-    <row r="90" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:26" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B90" s="12"/>
       <c r="C90" s="13"/>
       <c r="I90" s="12"/>
       <c r="J90" s="14"/>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.35">
       <c r="C91" s="73"/>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>617</v>
       </c>
@@ -7071,7 +7438,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>618</v>
       </c>
@@ -7088,7 +7455,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>625</v>
       </c>
@@ -7105,7 +7472,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="95" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>639</v>
       </c>
@@ -7124,7 +7491,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="96" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B96" s="11"/>
       <c r="D96" t="s">
         <v>637</v>
@@ -7575,8 +7942,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="V36:Z55">
-    <sortCondition ref="V36:V55" customList="GetArticles,GetReducedArticles,GetArticlesWithPriceChatty,GetArticlesWithPriceBulky"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="V68:Z82">
+    <sortCondition ref="V68:V82" customList="GetArticles,GetReducedArticles,GetArticlesWithPriceChatty,GetArticlesWithPriceBulky"/>
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>